<commit_message>
removed bins and objs
</commit_message>
<xml_diff>
--- a/TestResults/Deploy_Michael.Richter 2016-07-22 16_02_51/Out/Template2.xlsx
+++ b/TestResults/Deploy_Michael.Richter 2016-07-22 16_02_51/Out/Template2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Course" sheetId="1" r:id="rId1"/>
@@ -678,13 +678,13 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -698,7 +698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
@@ -719,12 +719,12 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="6" width="12.85546875" customWidth="1"/>
+    <col min="1" max="6" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -744,7 +744,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -774,18 +774,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="11" width="5" customWidth="1"/>
-    <col min="12" max="12" width="7.140625" customWidth="1"/>
+    <col min="12" max="12" width="7.1796875" customWidth="1"/>
     <col min="13" max="21" width="5" customWidth="1"/>
-    <col min="22" max="23" width="7.140625" customWidth="1"/>
+    <col min="22" max="23" width="7.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:23" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -846,7 +848,7 @@
       </c>
       <c r="V2" s="26"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -917,7 +919,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -978,7 +980,7 @@
       </c>
       <c r="V4" s="14"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1049,7 +1051,7 @@
         <v>5486</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="3.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C6" s="11"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -1071,45 +1073,81 @@
       <c r="U6" s="8"/>
       <c r="V6" s="16"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7">
-        <v>32.200000762939453</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="C7" s="9">
+        <v>3</v>
+      </c>
+      <c r="D7" s="4">
+        <v>4</v>
+      </c>
+      <c r="E7" s="4">
+        <v>4</v>
+      </c>
+      <c r="F7" s="4">
+        <v>5</v>
+      </c>
+      <c r="G7" s="4">
+        <v>4</v>
+      </c>
+      <c r="H7" s="4">
+        <v>3</v>
+      </c>
+      <c r="I7" s="4">
+        <v>3</v>
+      </c>
+      <c r="J7" s="4">
+        <v>5</v>
+      </c>
+      <c r="K7" s="6">
+        <v>4</v>
+      </c>
       <c r="L7" s="13">
         <f>SUM(C7:K7)</f>
-        <v>0</v>
-      </c>
-      <c r="M7" s="9"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="M7" s="9">
+        <v>4</v>
+      </c>
+      <c r="N7" s="4">
+        <v>5</v>
+      </c>
+      <c r="O7" s="4">
+        <v>3</v>
+      </c>
+      <c r="P7" s="4">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>3</v>
+      </c>
+      <c r="R7" s="4">
+        <v>4</v>
+      </c>
+      <c r="S7" s="4">
+        <v>4</v>
+      </c>
+      <c r="T7" s="4">
+        <v>4</v>
+      </c>
+      <c r="U7" s="6">
+        <v>3</v>
+      </c>
       <c r="V7" s="13">
         <f>SUM(M7:U7)</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="W7" s="12">
         <f>L7+V7</f>
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="3.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C8" s="11"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
@@ -1131,423 +1169,423 @@
       <c r="U8" s="8"/>
       <c r="V8" s="17"/>
     </row>
-    <row r="9" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="C9" s="11">
-        <f>$B$7-C$4</f>
-        <v>15.200000762939453</v>
+        <f t="shared" ref="C9:K9" si="0">$B$7-C$4</f>
+        <v>15</v>
       </c>
       <c r="D9" s="8">
-        <f>$B$7-D$4</f>
-        <v>25.200000762939453</v>
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
       <c r="E9" s="8">
-        <f>$B$7-E$4</f>
-        <v>29.200000762939453</v>
+        <f t="shared" si="0"/>
+        <v>29</v>
       </c>
       <c r="F9" s="8">
-        <f>$B$7-F$4</f>
-        <v>27.200000762939453</v>
+        <f t="shared" si="0"/>
+        <v>27</v>
       </c>
       <c r="G9" s="8">
-        <f>$B$7-G$4</f>
-        <v>19.200000762939453</v>
+        <f t="shared" si="0"/>
+        <v>19</v>
       </c>
       <c r="H9" s="8">
-        <f>$B$7-H$4</f>
-        <v>21.200000762939453</v>
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
       <c r="I9" s="8">
-        <f>$B$7-I$4</f>
-        <v>23.200000762939453</v>
+        <f t="shared" si="0"/>
+        <v>23</v>
       </c>
       <c r="J9" s="8">
-        <f>$B$7-J$4</f>
-        <v>31.200000762939453</v>
+        <f t="shared" si="0"/>
+        <v>31</v>
       </c>
       <c r="K9" s="8">
-        <f>$B$7-K$4</f>
-        <v>17.200000762939453</v>
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
       <c r="L9" s="18"/>
       <c r="M9" s="11">
-        <f>$B$7-M$4</f>
-        <v>16.200000762939453</v>
+        <f t="shared" ref="M9:U9" si="1">$B$7-M$4</f>
+        <v>16</v>
       </c>
       <c r="N9" s="8">
-        <f>$B$7-N$4</f>
-        <v>28.200000762939453</v>
+        <f t="shared" si="1"/>
+        <v>28</v>
       </c>
       <c r="O9" s="8">
-        <f>$B$7-O$4</f>
-        <v>30.200000762939453</v>
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="P9" s="8">
-        <f>$B$7-P$4</f>
-        <v>20.200000762939453</v>
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
       <c r="Q9" s="8">
-        <f>$B$7-Q$4</f>
-        <v>14.200000762939453</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="R9" s="8">
-        <f>$B$7-R$4</f>
-        <v>22.200000762939453</v>
+        <f t="shared" si="1"/>
+        <v>22</v>
       </c>
       <c r="S9" s="8">
-        <f>$B$7-S$4</f>
-        <v>26.200000762939453</v>
+        <f t="shared" si="1"/>
+        <v>26</v>
       </c>
       <c r="T9" s="8">
-        <f>$B$7-T$4</f>
-        <v>24.200000762939453</v>
+        <f t="shared" si="1"/>
+        <v>24</v>
       </c>
       <c r="U9" s="8">
-        <f>$B$7-U$4</f>
-        <v>18.200000762939453</v>
+        <f t="shared" si="1"/>
+        <v>18</v>
       </c>
       <c r="V9" s="18"/>
     </row>
-    <row r="10" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="C10" s="11">
-        <f>IF(C9&lt;0,0,IF(C9&lt;18,1,IF(C9&lt;36,2,3)))</f>
+        <f t="shared" ref="C10:K10" si="2">IF(C9&lt;0,0,IF(C9&lt;18,1,IF(C9&lt;36,2,3)))</f>
         <v>1</v>
       </c>
       <c r="D10" s="8">
-        <f>IF(D9&lt;0,0,IF(D9&lt;18,1,IF(D9&lt;36,2,3)))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E10" s="8">
-        <f>IF(E9&lt;0,0,IF(E9&lt;18,1,IF(E9&lt;36,2,3)))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="F10" s="8">
-        <f>IF(F9&lt;0,0,IF(F9&lt;18,1,IF(F9&lt;36,2,3)))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="G10" s="8">
-        <f>IF(G9&lt;0,0,IF(G9&lt;18,1,IF(G9&lt;36,2,3)))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H10" s="8">
-        <f>IF(H9&lt;0,0,IF(H9&lt;18,1,IF(H9&lt;36,2,3)))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I10" s="8">
-        <f>IF(I9&lt;0,0,IF(I9&lt;18,1,IF(I9&lt;36,2,3)))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J10" s="8">
-        <f>IF(J9&lt;0,0,IF(J9&lt;18,1,IF(J9&lt;36,2,3)))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K10" s="8">
-        <f>IF(K9&lt;0,0,IF(K9&lt;18,1,IF(K9&lt;36,2,3)))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L10" s="18"/>
       <c r="M10" s="11">
-        <f>IF(M9&lt;0,0,IF(M9&lt;18,1,IF(M9&lt;36,2,3)))</f>
+        <f t="shared" ref="M10:U10" si="3">IF(M9&lt;0,0,IF(M9&lt;18,1,IF(M9&lt;36,2,3)))</f>
         <v>1</v>
       </c>
       <c r="N10" s="8">
-        <f>IF(N9&lt;0,0,IF(N9&lt;18,1,IF(N9&lt;36,2,3)))</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="O10" s="8">
-        <f>IF(O9&lt;0,0,IF(O9&lt;18,1,IF(O9&lt;36,2,3)))</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="P10" s="8">
-        <f>IF(P9&lt;0,0,IF(P9&lt;18,1,IF(P9&lt;36,2,3)))</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="Q10" s="8">
-        <f>IF(Q9&lt;0,0,IF(Q9&lt;18,1,IF(Q9&lt;36,2,3)))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="R10" s="8">
-        <f>IF(R9&lt;0,0,IF(R9&lt;18,1,IF(R9&lt;36,2,3)))</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="S10" s="8">
-        <f>IF(S9&lt;0,0,IF(S9&lt;18,1,IF(S9&lt;36,2,3)))</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="T10" s="8">
-        <f>IF(T9&lt;0,0,IF(T9&lt;18,1,IF(T9&lt;36,2,3)))</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="U10" s="8">
-        <f>IF(U9&lt;0,0,IF(U9&lt;18,1,IF(U9&lt;36,2,3)))</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="V10" s="18"/>
     </row>
-    <row r="11" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="C11" s="11">
-        <f>C$3-C7</f>
-        <v>3</v>
+        <f t="shared" ref="C11:K11" si="4">C$3-C7</f>
+        <v>0</v>
       </c>
       <c r="D11" s="8">
-        <f>D$3-D7</f>
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="E11" s="8">
-        <f>E$3-E7</f>
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="F11" s="8">
-        <f>F$3-F7</f>
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="G11" s="8">
-        <f>G$3-G7</f>
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="H11" s="8">
-        <f>H$3-H7</f>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="I11" s="8">
-        <f>I$3-I7</f>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="J11" s="8">
-        <f>J$3-J7</f>
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="K11" s="8">
-        <f>K$3-K7</f>
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="L11" s="13">
         <f>SUM(C11:K11)</f>
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="M11" s="11">
-        <f>M$3-M7</f>
-        <v>4</v>
+        <f t="shared" ref="M11:U11" si="5">M$3-M7</f>
+        <v>0</v>
       </c>
       <c r="N11" s="8">
-        <f>N$3-N7</f>
-        <v>5</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="O11" s="8">
-        <f>O$3-O7</f>
-        <v>3</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="P11" s="8">
-        <f>P$3-P7</f>
-        <v>4</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="Q11" s="8">
-        <f>Q$3-Q7</f>
-        <v>3</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="R11" s="8">
-        <f>R$3-R7</f>
-        <v>4</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="S11" s="8">
-        <f>S$3-S7</f>
-        <v>4</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="T11" s="8">
-        <f>T$3-T7</f>
-        <v>4</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="U11" s="8">
-        <f>U$3-U7</f>
-        <v>3</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="V11" s="13">
         <f>SUM(M11:U11)</f>
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="W11" s="12">
         <f>L11+V11</f>
-        <v>69</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="9" t="str">
-        <f>IF(C7&lt;1,"",IF((2+C11+C10)&gt;-1,(2+C11+C10),0))</f>
-        <v/>
-      </c>
-      <c r="D12" s="4" t="str">
-        <f>IF(D7&lt;1,"",IF((2+D11+D10)&gt;-1,(2+D11+D10),0))</f>
-        <v/>
-      </c>
-      <c r="E12" s="4" t="str">
-        <f>IF(E7&lt;1,"",IF((2+E11+E10)&gt;-1,(2+E11+E10),0))</f>
-        <v/>
-      </c>
-      <c r="F12" s="4" t="str">
-        <f>IF(F7&lt;1,"",IF((2+F11+F10)&gt;-1,(2+F11+F10),0))</f>
-        <v/>
-      </c>
-      <c r="G12" s="4" t="str">
-        <f>IF(G7&lt;1,"",IF((2+G11+G10)&gt;-1,(2+G11+G10),0))</f>
-        <v/>
-      </c>
-      <c r="H12" s="4" t="str">
-        <f>IF(H7&lt;1,"",IF((2+H11+H10)&gt;-1,(2+H11+H10),0))</f>
-        <v/>
-      </c>
-      <c r="I12" s="4" t="str">
-        <f>IF(I7&lt;1,"",IF((2+I11+I10)&gt;-1,(2+I11+I10),0))</f>
-        <v/>
-      </c>
-      <c r="J12" s="4" t="str">
-        <f>IF(J7&lt;1,"",IF((2+J11+J10)&gt;-1,(2+J11+J10),0))</f>
-        <v/>
-      </c>
-      <c r="K12" s="6" t="str">
-        <f>IF(K7&lt;1,"",IF((2+K11+K10)&gt;-1,(2+K11+K10),0))</f>
-        <v/>
+      <c r="C12" s="9">
+        <f t="shared" ref="C12:K12" si="6">IF(C7&lt;1,"",IF((2+C11+C10)&gt;-1,(2+C11+C10),0))</f>
+        <v>3</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="H12" s="4">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="K12" s="6">
+        <f t="shared" si="6"/>
+        <v>3</v>
       </c>
       <c r="L12" s="13">
         <f>SUM(C12:K12)</f>
-        <v>0</v>
-      </c>
-      <c r="M12" s="9" t="str">
-        <f>IF(M7&lt;1,"",IF((2+M11+M10)&gt;-1,(2+M11+M10),0))</f>
-        <v/>
-      </c>
-      <c r="N12" s="4" t="str">
-        <f>IF(N7&lt;1,"",IF((2+N11+N10)&gt;-1,(2+N11+N10),0))</f>
-        <v/>
-      </c>
-      <c r="O12" s="4" t="str">
-        <f>IF(O7&lt;1,"",IF((2+O11+O10)&gt;-1,(2+O11+O10),0))</f>
-        <v/>
-      </c>
-      <c r="P12" s="4" t="str">
-        <f>IF(P7&lt;1,"",IF((2+P11+P10)&gt;-1,(2+P11+P10),0))</f>
-        <v/>
-      </c>
-      <c r="Q12" s="4" t="str">
-        <f>IF(Q7&lt;1,"",IF((2+Q11+Q10)&gt;-1,(2+Q11+Q10),0))</f>
-        <v/>
-      </c>
-      <c r="R12" s="4" t="str">
-        <f>IF(R7&lt;1,"",IF((2+R11+R10)&gt;-1,(2+R11+R10),0))</f>
-        <v/>
-      </c>
-      <c r="S12" s="4" t="str">
-        <f>IF(S7&lt;1,"",IF((2+S11+S10)&gt;-1,(2+S11+S10),0))</f>
-        <v/>
-      </c>
-      <c r="T12" s="4" t="str">
-        <f>IF(T7&lt;1,"",IF((2+T11+T10)&gt;-1,(2+T11+T10),0))</f>
-        <v/>
-      </c>
-      <c r="U12" s="6" t="str">
-        <f>IF(U7&lt;1,"",IF((2+U11+U10)&gt;-1,(2+U11+U10),0))</f>
-        <v/>
+        <v>34</v>
+      </c>
+      <c r="M12" s="9">
+        <f t="shared" ref="M12:U12" si="7">IF(M7&lt;1,"",IF((2+M11+M10)&gt;-1,(2+M11+M10),0))</f>
+        <v>3</v>
+      </c>
+      <c r="N12" s="4">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="O12" s="4">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="P12" s="4">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="Q12" s="4">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="R12" s="4">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="S12" s="4">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="T12" s="4">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="U12" s="6">
+        <f t="shared" si="7"/>
+        <v>4</v>
       </c>
       <c r="V12" s="13">
         <f>SUM(M12:U12)</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="W12" s="12">
         <f>L12+V12</f>
-        <v>0</v>
+        <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="19" t="str">
-        <f>IF(C7&lt;1,"",IF((2+C11)&gt;-1,(2+C11),0))</f>
-        <v/>
-      </c>
-      <c r="D13" s="20" t="str">
-        <f>IF(D7&lt;1,"",IF((2+D11)&gt;-1,(2+D11),0))</f>
-        <v/>
-      </c>
-      <c r="E13" s="20" t="str">
-        <f>IF(E7&lt;1,"",IF((2+E11)&gt;-1,(2+E11),0))</f>
-        <v/>
-      </c>
-      <c r="F13" s="20" t="str">
-        <f>IF(F7&lt;1,"",IF((2+F11)&gt;-1,(2+F11),0))</f>
-        <v/>
-      </c>
-      <c r="G13" s="20" t="str">
-        <f>IF(G7&lt;1,"",IF((2+G11)&gt;-1,(2+G11),0))</f>
-        <v/>
-      </c>
-      <c r="H13" s="20" t="str">
-        <f>IF(H7&lt;1,"",IF((2+H11)&gt;-1,(2+H11),0))</f>
-        <v/>
-      </c>
-      <c r="I13" s="20" t="str">
-        <f>IF(I7&lt;1,"",IF((2+I11)&gt;-1,(2+I11),0))</f>
-        <v/>
-      </c>
-      <c r="J13" s="20" t="str">
-        <f>IF(J7&lt;1,"",IF((2+J11)&gt;-1,(2+J11),0))</f>
-        <v/>
-      </c>
-      <c r="K13" s="21" t="str">
-        <f>IF(K7&lt;1,"",IF((2+K11)&gt;-1,(2+K11),0))</f>
-        <v/>
+      <c r="C13" s="19">
+        <f t="shared" ref="C13:K13" si="8">IF(C7&lt;1,"",IF((2+C11)&gt;-1,(2+C11),0))</f>
+        <v>2</v>
+      </c>
+      <c r="D13" s="20">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E13" s="20">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="F13" s="20">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="G13" s="20">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="H13" s="20">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="I13" s="20">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="J13" s="20">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="K13" s="21">
+        <f t="shared" si="8"/>
+        <v>2</v>
       </c>
       <c r="L13" s="22">
         <f>SUM(C13:K13)</f>
-        <v>0</v>
-      </c>
-      <c r="M13" s="19" t="str">
-        <f>IF(M7&lt;1,"",IF((2+M11)&gt;-1,(2+M11),0))</f>
-        <v/>
-      </c>
-      <c r="N13" s="20" t="str">
-        <f>IF(N7&lt;1,"",IF((2+N11)&gt;-1,(2+N11),0))</f>
-        <v/>
-      </c>
-      <c r="O13" s="20" t="str">
-        <f>IF(O7&lt;1,"",IF((2+O11)&gt;-1,(2+O11),0))</f>
-        <v/>
-      </c>
-      <c r="P13" s="20" t="str">
-        <f>IF(P7&lt;1,"",IF((2+P11)&gt;-1,(2+P11),0))</f>
-        <v/>
-      </c>
-      <c r="Q13" s="20" t="str">
-        <f>IF(Q7&lt;1,"",IF((2+Q11)&gt;-1,(2+Q11),0))</f>
-        <v/>
-      </c>
-      <c r="R13" s="20" t="str">
-        <f>IF(R7&lt;1,"",IF((2+R11)&gt;-1,(2+R11),0))</f>
-        <v/>
-      </c>
-      <c r="S13" s="20" t="str">
-        <f>IF(S7&lt;1,"",IF((2+S11)&gt;-1,(2+S11),0))</f>
-        <v/>
-      </c>
-      <c r="T13" s="20" t="str">
-        <f>IF(T7&lt;1,"",IF((2+T11)&gt;-1,(2+T11),0))</f>
-        <v/>
-      </c>
-      <c r="U13" s="21" t="str">
-        <f>IF(U7&lt;1,"",IF((2+U11)&gt;-1,(2+U11),0))</f>
-        <v/>
+        <v>18</v>
+      </c>
+      <c r="M13" s="19">
+        <f t="shared" ref="M13:U13" si="9">IF(M7&lt;1,"",IF((2+M11)&gt;-1,(2+M11),0))</f>
+        <v>2</v>
+      </c>
+      <c r="N13" s="20">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="O13" s="20">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="P13" s="20">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="Q13" s="20">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="R13" s="20">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="S13" s="20">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="T13" s="20">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="U13" s="21">
+        <f t="shared" si="9"/>
+        <v>2</v>
       </c>
       <c r="V13" s="22">
         <f>SUM(M13:U13)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="W13" s="12">
         <f>L13+V13</f>
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:23" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1562,7 +1600,7 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>